<commit_message>
add API Web to code
</commit_message>
<xml_diff>
--- a/ITEM_INFORMATION.xlsx
+++ b/ITEM_INFORMATION.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Estore\MiddlewareTool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936B8177-3D2D-4B90-8391-C33C5BF15D26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B2AE6C-383A-410B-BE54-DFDEA8DCA2BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CC377776-0D16-4C4A-A8AE-5191BF7205B1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CC377776-0D16-4C4A-A8AE-5191BF7205B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="73">
   <si>
     <t>032</t>
   </si>
@@ -232,6 +232,18 @@
   </si>
   <si>
     <t>HT02X</t>
+  </si>
+  <si>
+    <t>015</t>
+  </si>
+  <si>
+    <t>Combo 2 chai đỏ 3 chai xanh</t>
+  </si>
+  <si>
+    <t>016</t>
+  </si>
+  <si>
+    <t>combo 3 chai đỏ 2 chai xanh</t>
   </si>
 </sst>
 </file>
@@ -340,7 +352,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -367,6 +379,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -682,24 +696,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{388D4085-4A68-B840-8338-57C1E8076B76}">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="67.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="44" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.69921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.75" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>14</v>
       </c>
@@ -713,7 +727,7 @@
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>59</v>
       </c>
@@ -739,7 +753,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -765,7 +779,7 @@
         <v>170000</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -791,7 +805,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
@@ -817,7 +831,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>2</v>
       </c>
@@ -843,7 +857,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>3</v>
       </c>
@@ -869,7 +883,7 @@
         <v>170000</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>3</v>
       </c>
@@ -895,7 +909,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -921,7 +935,7 @@
         <v>1250000</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -947,7 +961,7 @@
         <v>1350000</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -973,7 +987,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -999,7 +1013,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>8</v>
       </c>
@@ -1025,7 +1039,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>8</v>
       </c>
@@ -1051,7 +1065,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>9</v>
       </c>
@@ -1077,7 +1091,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>9</v>
       </c>
@@ -1103,7 +1117,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>35</v>
       </c>
@@ -1129,7 +1143,7 @@
         <v>170000</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>36</v>
       </c>
@@ -1155,7 +1169,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>37</v>
       </c>
@@ -1181,7 +1195,7 @@
         <v>170000</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>38</v>
       </c>
@@ -1207,7 +1221,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>39</v>
       </c>
@@ -1233,7 +1247,7 @@
         <v>170000</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>39</v>
       </c>
@@ -1259,7 +1273,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>40</v>
       </c>
@@ -1285,7 +1299,7 @@
         <v>170000</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>40</v>
       </c>
@@ -1311,7 +1325,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>45</v>
       </c>
@@ -1337,7 +1351,7 @@
         <v>227273</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>49</v>
       </c>
@@ -1363,7 +1377,7 @@
         <v>160000</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>50</v>
       </c>
@@ -1389,7 +1403,7 @@
         <v>160000</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>51</v>
       </c>
@@ -1413,6 +1427,110 @@
       </c>
       <c r="H28" s="5">
         <v>160000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="13">
+        <v>1</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="13">
+        <v>2</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H29" s="13">
+        <v>170000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" s="13">
+        <v>1</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30" s="13">
+        <v>3</v>
+      </c>
+      <c r="G30" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H30" s="13">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" s="13">
+        <v>1</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="13">
+        <v>3</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H31" s="13">
+        <v>170000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" s="13">
+        <v>1</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" s="13">
+        <v>2</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H32" s="13">
+        <v>150000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor show information order from web
</commit_message>
<xml_diff>
--- a/ITEM_INFORMATION.xlsx
+++ b/ITEM_INFORMATION.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Estore\MiddlewareTool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B2AE6C-383A-410B-BE54-DFDEA8DCA2BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048EEA42-74DF-4DF1-8D55-D845F4576034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CC377776-0D16-4C4A-A8AE-5191BF7205B1}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{CC377776-0D16-4C4A-A8AE-5191BF7205B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -373,14 +373,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -699,7 +699,7 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -714,18 +714,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="10" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1430,106 +1430,106 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C29" s="13">
-        <v>1</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="E29" s="13" t="s">
+      <c r="C29" s="11">
+        <v>1</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F29" s="13">
+      <c r="F29" s="11">
         <v>2</v>
       </c>
-      <c r="G29" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="H29" s="13">
+      <c r="G29" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H29" s="11">
         <v>170000</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C30" s="13">
-        <v>1</v>
-      </c>
-      <c r="D30" s="12" t="s">
+      <c r="C30" s="11">
+        <v>1</v>
+      </c>
+      <c r="D30" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="E30" s="13" t="s">
+      <c r="E30" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F30" s="13">
+      <c r="F30" s="11">
         <v>3</v>
       </c>
-      <c r="G30" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="H30" s="13">
+      <c r="G30" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H30" s="11">
         <v>150000</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
+      <c r="A31" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C31" s="13">
-        <v>1</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="E31" s="13" t="s">
+      <c r="C31" s="11">
+        <v>1</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F31" s="13">
+      <c r="F31" s="11">
         <v>3</v>
       </c>
-      <c r="G31" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="H31" s="13">
+      <c r="G31" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H31" s="11">
         <v>170000</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="12" t="s">
+      <c r="A32" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C32" s="13">
-        <v>1</v>
-      </c>
-      <c r="D32" s="12" t="s">
+      <c r="C32" s="11">
+        <v>1</v>
+      </c>
+      <c r="D32" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="E32" s="13" t="s">
+      <c r="E32" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F32" s="13">
+      <c r="F32" s="11">
         <v>2</v>
       </c>
-      <c r="G32" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="H32" s="13">
+      <c r="G32" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H32" s="11">
         <v>150000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update code version issue distinct calculate for Lazada
</commit_message>
<xml_diff>
--- a/ITEM_INFORMATION.xlsx
+++ b/ITEM_INFORMATION.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Estore\MiddlewareTool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048EEA42-74DF-4DF1-8D55-D845F4576034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F3039C-A801-489D-84C8-41A2A6BF22A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{CC377776-0D16-4C4A-A8AE-5191BF7205B1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{CC377776-0D16-4C4A-A8AE-5191BF7205B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="95">
   <si>
     <t>032</t>
   </si>
@@ -244,13 +244,79 @@
   </si>
   <si>
     <t>combo 3 chai đỏ 2 chai xanh</t>
+  </si>
+  <si>
+    <t>Combo 5 chai đỏ</t>
+  </si>
+  <si>
+    <t>Combo 5 chai xanh</t>
+  </si>
+  <si>
+    <t>UM01</t>
+  </si>
+  <si>
+    <t>Son ủ môi</t>
+  </si>
+  <si>
+    <t>CL01</t>
+  </si>
+  <si>
+    <t>Cù là húng quế</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cái </t>
+  </si>
+  <si>
+    <t>DL01</t>
+  </si>
+  <si>
+    <t>Combo du lịch</t>
+  </si>
+  <si>
+    <t>Bộ</t>
+  </si>
+  <si>
+    <t>NH01</t>
+  </si>
+  <si>
+    <t>Nước hoa nhài</t>
+  </si>
+  <si>
+    <t>Lọ</t>
+  </si>
+  <si>
+    <t>MN01</t>
+  </si>
+  <si>
+    <t>Mặt nạ hoa nhài</t>
+  </si>
+  <si>
+    <t>053</t>
+  </si>
+  <si>
+    <t>054</t>
+  </si>
+  <si>
+    <t>CD01</t>
+  </si>
+  <si>
+    <t>Gel đắp thảo dược (hũ 50gr)</t>
+  </si>
+  <si>
+    <t>Giá gốc combo</t>
+  </si>
+  <si>
+    <t>UMT01</t>
+  </si>
+  <si>
+    <t>Son ủ môi (hàng tặng)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -264,6 +330,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0451A5"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -298,7 +370,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -347,12 +419,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -375,12 +467,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -696,38 +803,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{388D4085-4A68-B840-8338-57C1E8076B76}">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="67.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.58203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="44" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.75" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="12" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>59</v>
       </c>
@@ -752,8 +860,11 @@
       <c r="H2" s="4" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -778,8 +889,11 @@
       <c r="H3" s="1">
         <v>170000</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="1">
+        <v>170000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -804,60 +918,69 @@
       <c r="H4" s="1">
         <v>150000</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="I4" s="1">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="C5" s="19">
+        <v>1</v>
+      </c>
+      <c r="D5" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="4">
         <v>2</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="1">
+      <c r="G5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="4">
         <v>50000</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="I5" s="4">
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="5">
-        <v>1</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="C6" s="19">
+        <v>1</v>
+      </c>
+      <c r="D6" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="4">
         <v>3</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="1">
+      <c r="G6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="4">
         <v>50000</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="4">
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>3</v>
       </c>
@@ -882,8 +1005,11 @@
       <c r="H7" s="1">
         <v>170000</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="1">
+        <v>490000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>3</v>
       </c>
@@ -908,8 +1034,11 @@
       <c r="H8" s="1">
         <v>150000</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="1">
+        <v>490000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -934,8 +1063,11 @@
       <c r="H9" s="1">
         <v>1250000</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="1">
+        <v>1250000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -960,8 +1092,11 @@
       <c r="H10" s="1">
         <v>1350000</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="1">
+        <v>1350000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -986,8 +1121,11 @@
       <c r="H11" s="1">
         <v>20000</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="1">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -1012,8 +1150,11 @@
       <c r="H12" s="1">
         <v>20000</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="1">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
         <v>8</v>
       </c>
@@ -1036,10 +1177,13 @@
         <v>21</v>
       </c>
       <c r="H13" s="1">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>100000</v>
+      </c>
+      <c r="I13" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
         <v>8</v>
       </c>
@@ -1062,10 +1206,13 @@
         <v>21</v>
       </c>
       <c r="H14" s="1">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>100000</v>
+      </c>
+      <c r="I14" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
         <v>9</v>
       </c>
@@ -1090,8 +1237,11 @@
       <c r="H15" s="1">
         <v>20000</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" s="1">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
         <v>9</v>
       </c>
@@ -1116,8 +1266,11 @@
       <c r="H16" s="1">
         <v>20000</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="1">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>35</v>
       </c>
@@ -1142,8 +1295,11 @@
       <c r="H17" s="1">
         <v>170000</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="1">
+        <v>340000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>36</v>
       </c>
@@ -1168,8 +1324,11 @@
       <c r="H18" s="1">
         <v>150000</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="1">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>37</v>
       </c>
@@ -1194,8 +1353,11 @@
       <c r="H19" s="1">
         <v>170000</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="1">
+        <v>510000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>38</v>
       </c>
@@ -1220,8 +1382,11 @@
       <c r="H20" s="1">
         <v>150000</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="1">
+        <v>450000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
         <v>39</v>
       </c>
@@ -1246,8 +1411,11 @@
       <c r="H21" s="1">
         <v>170000</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" s="1">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
         <v>39</v>
       </c>
@@ -1272,8 +1440,11 @@
       <c r="H22" s="1">
         <v>150000</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" s="1">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
         <v>40</v>
       </c>
@@ -1298,8 +1469,11 @@
       <c r="H23" s="1">
         <v>170000</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23" s="1">
+        <v>170000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
         <v>40</v>
       </c>
@@ -1324,8 +1498,11 @@
       <c r="H24" s="1">
         <v>150000</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24" s="1">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>45</v>
       </c>
@@ -1350,8 +1527,11 @@
       <c r="H25" s="1">
         <v>227273</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25" s="1">
+        <v>227273</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>49</v>
       </c>
@@ -1376,8 +1556,11 @@
       <c r="H26" s="1">
         <v>160000</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26" s="1">
+        <v>160000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>50</v>
       </c>
@@ -1402,8 +1585,11 @@
       <c r="H27" s="5">
         <v>160000</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27" s="5">
+        <v>160000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>51</v>
       </c>
@@ -1428,8 +1614,11 @@
       <c r="H28" s="5">
         <v>160000</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28" s="5">
+        <v>160000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="10" t="s">
         <v>69</v>
       </c>
@@ -1454,8 +1643,11 @@
       <c r="H29" s="11">
         <v>170000</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29" s="11">
+        <v>170000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="10" t="s">
         <v>69</v>
       </c>
@@ -1480,8 +1672,11 @@
       <c r="H30" s="11">
         <v>150000</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30" s="11">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="10" t="s">
         <v>71</v>
       </c>
@@ -1506,8 +1701,11 @@
       <c r="H31" s="11">
         <v>170000</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31" s="11">
+        <v>170000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="10" t="s">
         <v>71</v>
       </c>
@@ -1532,11 +1730,275 @@
       <c r="H32" s="11">
         <v>150000</v>
       </c>
+      <c r="I32" s="11">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B33" t="s">
+        <v>73</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33">
+        <v>3</v>
+      </c>
+      <c r="G33" t="s">
+        <v>19</v>
+      </c>
+      <c r="H33">
+        <v>170000</v>
+      </c>
+      <c r="I33">
+        <v>170000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B34" t="s">
+        <v>74</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E34" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34">
+        <v>2</v>
+      </c>
+      <c r="G34" t="s">
+        <v>19</v>
+      </c>
+      <c r="H34">
+        <v>150000</v>
+      </c>
+      <c r="I34">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" t="s">
+        <v>76</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35" t="s">
+        <v>75</v>
+      </c>
+      <c r="E35" t="s">
+        <v>76</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35" t="s">
+        <v>47</v>
+      </c>
+      <c r="H35">
+        <v>104545</v>
+      </c>
+      <c r="I35">
+        <v>104545</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>77</v>
+      </c>
+      <c r="B36" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36" t="s">
+        <v>77</v>
+      </c>
+      <c r="E36" t="s">
+        <v>78</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36" t="s">
+        <v>79</v>
+      </c>
+      <c r="H36">
+        <v>31818</v>
+      </c>
+      <c r="I36">
+        <v>31818</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37" t="s">
+        <v>80</v>
+      </c>
+      <c r="E37" t="s">
+        <v>81</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37" t="s">
+        <v>82</v>
+      </c>
+      <c r="H37">
+        <v>268182</v>
+      </c>
+      <c r="I37">
+        <v>268182</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>83</v>
+      </c>
+      <c r="B38" t="s">
+        <v>84</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
+        <v>83</v>
+      </c>
+      <c r="E38" t="s">
+        <v>84</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38" t="s">
+        <v>85</v>
+      </c>
+      <c r="H38">
+        <v>140909</v>
+      </c>
+      <c r="I38">
+        <v>140909</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>86</v>
+      </c>
+      <c r="B39" t="s">
+        <v>87</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
+        <v>86</v>
+      </c>
+      <c r="E39" t="s">
+        <v>87</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="G39" t="s">
+        <v>19</v>
+      </c>
+      <c r="H39">
+        <v>222727</v>
+      </c>
+      <c r="I39">
+        <v>222727</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A40" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H40">
+        <v>183000</v>
+      </c>
+      <c r="I40">
+        <v>183000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>93</v>
+      </c>
+      <c r="B41" t="s">
+        <v>94</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41" t="s">
+        <v>93</v>
+      </c>
+      <c r="E41" t="s">
+        <v>94</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+      <c r="G41" t="s">
+        <v>47</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="D1:H1"/>
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix error read SKU with excel file at web at product detail, and remove note discount in November
</commit_message>
<xml_diff>
--- a/ITEM_INFORMATION.xlsx
+++ b/ITEM_INFORMATION.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Estore\MiddlewareTool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F3039C-A801-489D-84C8-41A2A6BF22A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45086ECC-9268-48CA-A761-3AC9032F5881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{CC377776-0D16-4C4A-A8AE-5191BF7205B1}"/>
+    <workbookView xWindow="57480" yWindow="2130" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{CC377776-0D16-4C4A-A8AE-5191BF7205B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Giải thích" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="104">
   <si>
     <t>032</t>
   </si>
@@ -69,12 +70,6 @@
     <t>Set quà tặng</t>
   </si>
   <si>
-    <t>TRÊN SÀN</t>
-  </si>
-  <si>
-    <t>TRÊN HÓA ĐƠN</t>
-  </si>
-  <si>
     <t>Giang's Cao xoa thảo dược 15ml (chai đỏ)</t>
   </si>
   <si>
@@ -222,9 +217,6 @@
     <t>PRODUCT_QUANTITY</t>
   </si>
   <si>
-    <t xml:space="preserve">UNIT </t>
-  </si>
-  <si>
     <t>PRICE_NOT_VAT</t>
   </si>
   <si>
@@ -310,13 +302,87 @@
   </si>
   <si>
     <t>Son ủ môi (hàng tặng)</t>
+  </si>
+  <si>
+    <t>UNIT</t>
+  </si>
+  <si>
+    <t>PRODUCT_TITLE</t>
+  </si>
+  <si>
+    <t>TRÊN SÀN TMĐT/WEB</t>
+  </si>
+  <si>
+    <t>TRÊN HÓA ĐƠN/MISA</t>
+  </si>
+  <si>
+    <t>Tên sản phẩm</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mã sản phẩm sku </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CHA</t>
+    </r>
+  </si>
+  <si>
+    <t>Số lượng sản phẩm
+mặc định</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mã sản phẩm sku </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CON</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mã sản phẩm sku </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CON
+trên Misa</t>
+    </r>
+  </si>
+  <si>
+    <t>Số lượng sản phẩm</t>
+  </si>
+  <si>
+    <t>Đơn vị</t>
+  </si>
+  <si>
+    <t>Giá chưa thuế</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -336,6 +402,13 @@
       <color rgb="FF0451A5"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -370,7 +443,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -439,12 +512,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -471,15 +575,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -488,6 +583,24 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -803,10 +916,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{388D4085-4A68-B840-8338-57C1E8076B76}">
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -815,56 +928,61 @@
     <col min="2" max="2" width="67.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.58203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="E2" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="H2" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J2" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -877,23 +995,26 @@
       <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="1">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="1">
-        <v>170000</v>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="I3" s="1">
         <v>170000</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J3" s="1">
+        <v>170000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -906,86 +1027,95 @@
       <c r="D4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="1">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="1">
-        <v>150000</v>
+      <c r="E4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="I4" s="1">
         <v>150000</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="18" t="s">
+      <c r="J4" s="1">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="19">
-        <v>1</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="C5" s="16">
+        <v>1</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="4">
+        <v>2</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="4">
+        <v>50000</v>
+      </c>
+      <c r="J5" s="4">
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="16">
+        <v>1</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="4">
-        <v>2</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="4">
+      <c r="G6" s="4">
+        <v>3</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="4">
         <v>50000</v>
       </c>
-      <c r="I5" s="4">
+      <c r="J6" s="4">
         <v>250000</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="19">
-        <v>1</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="4">
-        <v>3</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="4">
-        <v>50000</v>
-      </c>
-      <c r="I6" s="4">
-        <v>250000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C7" s="5">
         <v>1</v>
@@ -993,28 +1123,31 @@
       <c r="D7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G7" s="1">
         <v>2</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="1">
+      <c r="H7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="1">
         <v>170000</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J7" s="1">
         <v>490000</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C8" s="6">
         <v>1</v>
@@ -1022,28 +1155,31 @@
       <c r="D8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="1">
-        <v>1</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="1">
+      <c r="E8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="1">
         <v>150000</v>
       </c>
-      <c r="I8" s="1">
+      <c r="J8" s="1">
         <v>490000</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
@@ -1052,27 +1188,30 @@
         <v>4</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="1">
-        <v>1</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" s="1">
-        <v>1250000</v>
+        <v>4</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="I9" s="1">
         <v>1250000</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J9" s="1">
+        <v>1250000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C10" s="1">
         <v>1</v>
@@ -1081,27 +1220,30 @@
         <v>5</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="1">
-        <v>1</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="1">
-        <v>1350000</v>
+        <v>5</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="I10" s="1">
         <v>1350000</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J10" s="1">
+        <v>1350000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
@@ -1110,27 +1252,30 @@
         <v>6</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="1">
-        <v>1</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" s="1">
-        <v>20000</v>
+        <v>6</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="I11" s="1">
         <v>20000</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J11" s="1">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
@@ -1139,27 +1284,30 @@
         <v>7</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="1">
-        <v>1</v>
-      </c>
-      <c r="G12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H12" s="1">
-        <v>20000</v>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="I12" s="1">
         <v>20000</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J12" s="1">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C13" s="8">
         <v>1</v>
@@ -1168,27 +1316,30 @@
         <v>6</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="1">
+        <v>6</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="1">
         <v>5</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13" s="1">
-        <v>100000</v>
+      <c r="H13" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="I13" s="1">
         <v>100000</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J13" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C14" s="8">
         <v>1</v>
@@ -1197,27 +1348,30 @@
         <v>7</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" s="1">
+        <v>7</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="1">
         <v>5</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H14" s="1">
-        <v>100000</v>
+      <c r="H14" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="I14" s="1">
         <v>100000</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J14" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C15" s="8">
         <v>1</v>
@@ -1226,27 +1380,30 @@
         <v>6</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F15" s="1">
+        <v>6</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H15" s="1">
+      <c r="G15" s="1">
+        <v>20</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" s="1">
         <v>20000</v>
       </c>
-      <c r="I15" s="1">
+      <c r="J15" s="1">
         <v>400000</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C16" s="8">
         <v>1</v>
@@ -1255,27 +1412,30 @@
         <v>7</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" s="1">
+        <v>7</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="1">
         <v>20</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H16" s="1">
+      <c r="H16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I16" s="1">
         <v>20000</v>
       </c>
-      <c r="I16" s="1">
+      <c r="J16" s="1">
         <v>400000</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C17" s="1">
         <v>1</v>
@@ -1283,28 +1443,31 @@
       <c r="D17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="1">
+      <c r="G17" s="1">
         <v>2</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H17" s="1">
+      <c r="H17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="1">
         <v>170000</v>
       </c>
-      <c r="I17" s="1">
+      <c r="J17" s="1">
         <v>340000</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C18" s="1">
         <v>1</v>
@@ -1312,28 +1475,31 @@
       <c r="D18" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F18" s="1">
+      <c r="E18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="1">
         <v>2</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H18" s="1">
+      <c r="H18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="1">
         <v>150000</v>
       </c>
-      <c r="I18" s="1">
+      <c r="J18" s="1">
         <v>300000</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C19" s="1">
         <v>1</v>
@@ -1341,28 +1507,31 @@
       <c r="D19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F19" s="1">
+      <c r="G19" s="1">
         <v>3</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H19" s="1">
+      <c r="H19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" s="1">
         <v>170000</v>
       </c>
-      <c r="I19" s="1">
+      <c r="J19" s="1">
         <v>510000</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C20" s="1">
         <v>1</v>
@@ -1370,28 +1539,31 @@
       <c r="D20" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" s="1">
+      <c r="E20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="1">
         <v>3</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H20" s="1">
+      <c r="H20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="1">
         <v>150000</v>
       </c>
-      <c r="I20" s="1">
+      <c r="J20" s="1">
         <v>450000</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C21" s="8">
         <v>1</v>
@@ -1399,28 +1571,31 @@
       <c r="D21" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F21" s="1">
-        <v>1</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H21" s="1">
+      <c r="G21" s="1">
+        <v>1</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" s="1">
         <v>170000</v>
       </c>
-      <c r="I21" s="1">
+      <c r="J21" s="1">
         <v>500000</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C22" s="8">
         <v>1</v>
@@ -1428,28 +1603,31 @@
       <c r="D22" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F22" s="1">
+      <c r="E22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="1">
         <v>2</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H22" s="1">
+      <c r="H22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" s="1">
         <v>150000</v>
       </c>
-      <c r="I22" s="1">
+      <c r="J22" s="1">
         <v>500000</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C23" s="8">
         <v>1</v>
@@ -1457,28 +1635,31 @@
       <c r="D23" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="1">
-        <v>1</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H23" s="1">
-        <v>170000</v>
+      <c r="G23" s="1">
+        <v>1</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="I23" s="1">
         <v>170000</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J23" s="1">
+        <v>170000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C24" s="8">
         <v>1</v>
@@ -1486,144 +1667,159 @@
       <c r="D24" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F24" s="1">
-        <v>1</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H24" s="1">
-        <v>150000</v>
+      <c r="E24" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" s="1">
+        <v>1</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="I24" s="1">
         <v>150000</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J24" s="1">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G25" s="1">
+        <v>1</v>
+      </c>
+      <c r="H25" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="1">
-        <v>1</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F25" s="1">
-        <v>1</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H25" s="1">
-        <v>227273</v>
       </c>
       <c r="I25" s="1">
         <v>227273</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J25" s="1">
+        <v>227273</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C26" s="1">
         <v>1</v>
       </c>
       <c r="D26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F26" s="1">
-        <v>1</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H26" s="1">
-        <v>160000</v>
+      <c r="G26" s="1">
+        <v>1</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="I26" s="1">
         <v>160000</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J26" s="1">
+        <v>160000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C27" s="1">
         <v>1</v>
       </c>
       <c r="D27" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F27" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E27" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="F27" s="5">
-        <v>1</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H27" s="5">
-        <v>160000</v>
+      <c r="G27" s="5">
+        <v>1</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="I27" s="5">
         <v>160000</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J27" s="5">
+        <v>160000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+      <c r="D28" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C28" s="1">
-        <v>1</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>53</v>
-      </c>
       <c r="E28" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="F28" s="5">
-        <v>1</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H28" s="5">
-        <v>160000</v>
+        <v>51</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G28" s="5">
+        <v>1</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="I28" s="5">
         <v>160000</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J28" s="5">
+        <v>160000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="10" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C29" s="11">
         <v>1</v>
@@ -1631,28 +1827,31 @@
       <c r="D29" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E29" s="11" t="s">
+      <c r="E29" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F29" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F29" s="11">
+      <c r="G29" s="11">
         <v>2</v>
       </c>
-      <c r="G29" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H29" s="11">
-        <v>170000</v>
+      <c r="H29" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="I29" s="11">
         <v>170000</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J29" s="11">
+        <v>170000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="10" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C30" s="11">
         <v>1</v>
@@ -1660,28 +1859,31 @@
       <c r="D30" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="E30" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F30" s="11">
+      <c r="E30" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30" s="11">
         <v>3</v>
       </c>
-      <c r="G30" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H30" s="11">
-        <v>150000</v>
+      <c r="H30" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="I30" s="11">
         <v>150000</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J30" s="11">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="10" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C31" s="11">
         <v>1</v>
@@ -1689,28 +1891,31 @@
       <c r="D31" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E31" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F31" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F31" s="11">
+      <c r="G31" s="11">
         <v>3</v>
       </c>
-      <c r="G31" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H31" s="11">
-        <v>170000</v>
+      <c r="H31" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="I31" s="11">
         <v>170000</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J31" s="11">
+        <v>170000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="10" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C32" s="11">
         <v>1</v>
@@ -1718,28 +1923,31 @@
       <c r="D32" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="E32" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F32" s="11">
+      <c r="E32" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32" s="11">
         <v>2</v>
       </c>
-      <c r="G32" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H32" s="11">
-        <v>150000</v>
+      <c r="H32" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="I32" s="11">
         <v>150000</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J32" s="11">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="12" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B33" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -1747,28 +1955,31 @@
       <c r="D33" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="F33" t="s">
         <v>10</v>
       </c>
-      <c r="F33">
+      <c r="G33">
         <v>3</v>
       </c>
-      <c r="G33" t="s">
-        <v>19</v>
-      </c>
-      <c r="H33">
-        <v>170000</v>
+      <c r="H33" t="s">
+        <v>17</v>
       </c>
       <c r="I33">
         <v>170000</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J33">
+        <v>170000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="12" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B34" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -1776,230 +1987,362 @@
       <c r="D34" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="E34" t="s">
-        <v>17</v>
-      </c>
-      <c r="F34">
+      <c r="E34" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="F34" t="s">
+        <v>15</v>
+      </c>
+      <c r="G34">
         <v>2</v>
       </c>
-      <c r="G34" t="s">
-        <v>19</v>
-      </c>
-      <c r="H34">
-        <v>150000</v>
+      <c r="H34" t="s">
+        <v>17</v>
       </c>
       <c r="I34">
         <v>150000</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J34">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B35" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C35">
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E35" t="s">
-        <v>76</v>
-      </c>
-      <c r="F35">
-        <v>1</v>
-      </c>
-      <c r="G35" t="s">
-        <v>47</v>
-      </c>
-      <c r="H35">
-        <v>104545</v>
+        <v>72</v>
+      </c>
+      <c r="F35" t="s">
+        <v>73</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35" t="s">
+        <v>45</v>
       </c>
       <c r="I35">
         <v>104545</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J35">
+        <v>104545</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B36" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C36">
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E36" t="s">
-        <v>78</v>
-      </c>
-      <c r="F36">
-        <v>1</v>
-      </c>
-      <c r="G36" t="s">
-        <v>79</v>
-      </c>
-      <c r="H36">
-        <v>31818</v>
+        <v>74</v>
+      </c>
+      <c r="F36" t="s">
+        <v>75</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36" t="s">
+        <v>76</v>
       </c>
       <c r="I36">
         <v>31818</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J36">
+        <v>31818</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B37" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C37">
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E37" t="s">
-        <v>81</v>
-      </c>
-      <c r="F37">
-        <v>1</v>
-      </c>
-      <c r="G37" t="s">
-        <v>82</v>
-      </c>
-      <c r="H37">
-        <v>268182</v>
+        <v>77</v>
+      </c>
+      <c r="F37" t="s">
+        <v>78</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37" t="s">
+        <v>79</v>
       </c>
       <c r="I37">
         <v>268182</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J37">
+        <v>268182</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B38" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C38">
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E38" t="s">
-        <v>84</v>
-      </c>
-      <c r="F38">
-        <v>1</v>
-      </c>
-      <c r="G38" t="s">
-        <v>85</v>
-      </c>
-      <c r="H38">
-        <v>140909</v>
+        <v>80</v>
+      </c>
+      <c r="F38" t="s">
+        <v>81</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38" t="s">
+        <v>82</v>
       </c>
       <c r="I38">
         <v>140909</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J38">
+        <v>140909</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B39" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C39">
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E39" t="s">
-        <v>87</v>
-      </c>
-      <c r="F39">
-        <v>1</v>
-      </c>
-      <c r="G39" t="s">
-        <v>19</v>
-      </c>
-      <c r="H39">
-        <v>222727</v>
+        <v>83</v>
+      </c>
+      <c r="F39" t="s">
+        <v>84</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39" t="s">
+        <v>17</v>
       </c>
       <c r="I39">
         <v>222727</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J39">
+        <v>222727</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="13" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C40">
         <v>1</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E40" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="F40">
-        <v>1</v>
-      </c>
-      <c r="G40" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="H40">
-        <v>183000</v>
+        <v>87</v>
+      </c>
+      <c r="F40" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+      <c r="H40" s="13" t="s">
+        <v>17</v>
       </c>
       <c r="I40">
         <v>183000</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J40">
+        <v>183000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B41" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C41">
         <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E41" t="s">
-        <v>94</v>
-      </c>
-      <c r="F41">
-        <v>1</v>
-      </c>
-      <c r="G41" t="s">
-        <v>47</v>
-      </c>
-      <c r="H41">
-        <v>0</v>
+        <v>90</v>
+      </c>
+      <c r="F41" t="s">
+        <v>91</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="H41" t="s">
+        <v>45</v>
       </c>
       <c r="I41">
         <v>0</v>
       </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56457DB1-F414-4FF6-9027-221481BF110F}">
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.58203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="19.58203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.08203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.08203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.58203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="F3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="H3" t="s">
+        <v>102</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Change Sapo get in composite_fulfillment_status=fulfilled
</commit_message>
<xml_diff>
--- a/ITEM_INFORMATION.xlsx
+++ b/ITEM_INFORMATION.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Estore\MiddlewareTool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45086ECC-9268-48CA-A761-3AC9032F5881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40559228-E4BD-4838-881C-2F8EF19DF334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="2130" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{CC377776-0D16-4C4A-A8AE-5191BF7205B1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{CC377776-0D16-4C4A-A8AE-5191BF7205B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -583,9 +583,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -598,7 +595,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -918,8 +918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{388D4085-4A68-B840-8338-57C1E8076B76}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -935,13 +935,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="18" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="22" t="s">
         <v>95</v>
       </c>
       <c r="F1" s="23"/>
@@ -1760,8 +1760,8 @@
       <c r="C27" s="1">
         <v>1</v>
       </c>
-      <c r="D27" s="8" t="s">
-        <v>51</v>
+      <c r="D27" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>51</v>
@@ -2243,7 +2243,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56457DB1-F414-4FF6-9027-221481BF110F}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
@@ -2261,13 +2261,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="18" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="22" t="s">
         <v>95</v>
       </c>
       <c r="F1" s="23"/>
@@ -2315,25 +2315,25 @@
       <c r="B3" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="18" t="s">
         <v>98</v>
       </c>
       <c r="D3" t="s">
         <v>99</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="18" t="s">
         <v>100</v>
       </c>
       <c r="F3" t="s">
         <v>96</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="18" t="s">
         <v>101</v>
       </c>
       <c r="H3" t="s">
         <v>102</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="I3" s="18" t="s">
         <v>103</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix bug with the new version Middleware_v2.0_20250120
</commit_message>
<xml_diff>
--- a/ITEM_INFORMATION.xlsx
+++ b/ITEM_INFORMATION.xlsx
@@ -1,32 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Estore\MiddlewareTool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40559228-E4BD-4838-881C-2F8EF19DF334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB6C743-634B-4540-BF66-9D6ABE90DF45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{CC377776-0D16-4C4A-A8AE-5191BF7205B1}"/>
+    <workbookView xWindow="57480" yWindow="2130" windowWidth="29040" windowHeight="15720" xr2:uid="{CC377776-0D16-4C4A-A8AE-5191BF7205B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Giải thích" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="111">
   <si>
     <t>032</t>
   </si>
@@ -377,12 +386,33 @@
   <si>
     <t>Giá chưa thuế</t>
   </si>
+  <si>
+    <t>2NH01</t>
+  </si>
+  <si>
+    <t>COMBO 2 NƯỚC HOA NHÀI</t>
+  </si>
+  <si>
+    <t>3NH01</t>
+  </si>
+  <si>
+    <t>COMBO 3 NƯỚC HOA NHÀI</t>
+  </si>
+  <si>
+    <t>MAS1</t>
+  </si>
+  <si>
+    <t>Máy Massage Cổ vai gáy</t>
+  </si>
+  <si>
+    <t>Máy massage cổ dùng pin sạc 6D</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -406,6 +436,26 @@
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -544,11 +594,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -586,6 +637,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -602,7 +655,8 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{92F0FB6A-23FD-5A43-A969-F070261307DE}"/>
   </cellStyles>
@@ -916,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{388D4085-4A68-B840-8338-57C1E8076B76}">
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="67.5" bestFit="1" customWidth="1"/>
@@ -934,23 +988,23 @@
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="22" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="3" t="s">
         <v>57</v>
       </c>
@@ -982,7 +1036,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1014,7 +1068,7 @@
         <v>170000</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1046,7 +1100,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10">
       <c r="A5" s="15" t="s">
         <v>2</v>
       </c>
@@ -1078,7 +1132,7 @@
         <v>250000</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10">
       <c r="A6" s="15" t="s">
         <v>2</v>
       </c>
@@ -1110,7 +1164,7 @@
         <v>250000</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10">
       <c r="A7" s="7" t="s">
         <v>3</v>
       </c>
@@ -1142,7 +1196,7 @@
         <v>490000</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10">
       <c r="A8" s="7" t="s">
         <v>3</v>
       </c>
@@ -1174,7 +1228,7 @@
         <v>490000</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -1206,7 +1260,7 @@
         <v>1250000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -1232,13 +1286,13 @@
         <v>18</v>
       </c>
       <c r="I10" s="1">
-        <v>1350000</v>
+        <v>0</v>
       </c>
       <c r="J10" s="1">
-        <v>1350000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -1270,7 +1324,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -1302,7 +1356,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10">
       <c r="A13" s="8" t="s">
         <v>8</v>
       </c>
@@ -1334,7 +1388,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10">
       <c r="A14" s="8" t="s">
         <v>8</v>
       </c>
@@ -1366,7 +1420,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10">
       <c r="A15" s="8" t="s">
         <v>9</v>
       </c>
@@ -1398,7 +1452,7 @@
         <v>400000</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10">
       <c r="A16" s="8" t="s">
         <v>9</v>
       </c>
@@ -1430,7 +1484,7 @@
         <v>400000</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10">
       <c r="A17" s="2" t="s">
         <v>33</v>
       </c>
@@ -1462,7 +1516,7 @@
         <v>340000</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10">
       <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
@@ -1494,7 +1548,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10">
       <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
@@ -1526,7 +1580,7 @@
         <v>510000</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10">
       <c r="A20" s="2" t="s">
         <v>36</v>
       </c>
@@ -1558,7 +1612,7 @@
         <v>450000</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10">
       <c r="A21" s="9" t="s">
         <v>37</v>
       </c>
@@ -1590,7 +1644,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10">
       <c r="A22" s="9" t="s">
         <v>37</v>
       </c>
@@ -1622,7 +1676,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10">
       <c r="A23" s="9" t="s">
         <v>38</v>
       </c>
@@ -1654,7 +1708,7 @@
         <v>170000</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10">
       <c r="A24" s="9" t="s">
         <v>38</v>
       </c>
@@ -1686,7 +1740,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10">
       <c r="A25" s="1" t="s">
         <v>43</v>
       </c>
@@ -1718,7 +1772,7 @@
         <v>227273</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10">
       <c r="A26" s="1" t="s">
         <v>47</v>
       </c>
@@ -1750,7 +1804,7 @@
         <v>160000</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10">
       <c r="A27" s="1" t="s">
         <v>48</v>
       </c>
@@ -1782,7 +1836,7 @@
         <v>160000</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10">
       <c r="A28" s="1" t="s">
         <v>49</v>
       </c>
@@ -1814,7 +1868,7 @@
         <v>160000</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10">
       <c r="A29" s="10" t="s">
         <v>66</v>
       </c>
@@ -1846,7 +1900,7 @@
         <v>170000</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10">
       <c r="A30" s="10" t="s">
         <v>66</v>
       </c>
@@ -1878,7 +1932,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10">
       <c r="A31" s="10" t="s">
         <v>68</v>
       </c>
@@ -1910,7 +1964,7 @@
         <v>170000</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10">
       <c r="A32" s="10" t="s">
         <v>68</v>
       </c>
@@ -1942,7 +1996,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10">
       <c r="A33" s="12" t="s">
         <v>85</v>
       </c>
@@ -1974,7 +2028,7 @@
         <v>170000</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10">
       <c r="A34" s="12" t="s">
         <v>86</v>
       </c>
@@ -2006,7 +2060,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10">
       <c r="A35" t="s">
         <v>72</v>
       </c>
@@ -2038,7 +2092,7 @@
         <v>104545</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10">
       <c r="A36" t="s">
         <v>74</v>
       </c>
@@ -2070,7 +2124,7 @@
         <v>31818</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10">
       <c r="A37" t="s">
         <v>77</v>
       </c>
@@ -2102,7 +2156,7 @@
         <v>268182</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10">
       <c r="A38" t="s">
         <v>80</v>
       </c>
@@ -2134,7 +2188,7 @@
         <v>140909</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10">
       <c r="A39" t="s">
         <v>83</v>
       </c>
@@ -2166,7 +2220,7 @@
         <v>222727</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10">
       <c r="A40" s="13" t="s">
         <v>87</v>
       </c>
@@ -2198,7 +2252,7 @@
         <v>183000</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10">
       <c r="A41" t="s">
         <v>90</v>
       </c>
@@ -2228,6 +2282,103 @@
       </c>
       <c r="J41">
         <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="B42" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42" t="s">
+        <v>80</v>
+      </c>
+      <c r="E42" t="s">
+        <v>80</v>
+      </c>
+      <c r="F42" t="s">
+        <v>81</v>
+      </c>
+      <c r="G42">
+        <v>2</v>
+      </c>
+      <c r="H42" t="s">
+        <v>82</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="B43" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>80</v>
+      </c>
+      <c r="E43" t="s">
+        <v>80</v>
+      </c>
+      <c r="F43" t="s">
+        <v>81</v>
+      </c>
+      <c r="G43">
+        <v>3</v>
+      </c>
+      <c r="H43" t="s">
+        <v>82</v>
+      </c>
+      <c r="I43">
+        <v>140909</v>
+      </c>
+      <c r="J43">
+        <f>I43*3</f>
+        <v>422727</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" t="s">
+        <v>108</v>
+      </c>
+      <c r="B44" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44" t="s">
+        <v>108</v>
+      </c>
+      <c r="E44" t="s">
+        <v>108</v>
+      </c>
+      <c r="F44" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44" t="s">
+        <v>45</v>
+      </c>
+      <c r="I44">
+        <v>1150000</v>
+      </c>
+      <c r="J44">
+        <v>1150000</v>
       </c>
     </row>
   </sheetData>
@@ -2235,6 +2386,11 @@
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="E1:J1"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A42" r:id="rId1" display="https://caoxoaquoccoquocnghiep.mysapogo.com/admin/products/193913949/variants/315993725" xr:uid="{E680888A-8F33-4198-B5BF-F49F443CA594}"/>
+    <hyperlink ref="A43" r:id="rId2" display="https://caoxoaquoccoquocnghiep.mysapogo.com/admin/products/193913988/variants/315993781" xr:uid="{003B007F-9563-4499-B56C-636742EC6E46}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2247,7 +2403,7 @@
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.25" bestFit="1" customWidth="1"/>
@@ -2260,23 +2416,23 @@
     <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="22" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="3" t="s">
         <v>57</v>
       </c>
@@ -2308,7 +2464,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="31">
       <c r="A3" t="s">
         <v>97</v>
       </c>

</xml_diff>

<commit_message>
Update run multi thread
</commit_message>
<xml_diff>
--- a/ITEM_INFORMATION.xlsx
+++ b/ITEM_INFORMATION.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Estore\MiddlewareTool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB6C743-634B-4540-BF66-9D6ABE90DF45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9943D00-64E8-4BDE-BA65-B0C92D38B88C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="2130" windowWidth="29040" windowHeight="15720" xr2:uid="{CC377776-0D16-4C4A-A8AE-5191BF7205B1}"/>
   </bookViews>
@@ -972,8 +972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{388D4085-4A68-B840-8338-57C1E8076B76}">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
@@ -1783,7 +1783,7 @@
         <v>1</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>50</v>

</xml_diff>